<commit_message>
br08: skipped if term is dismissed br08: changed message specifying the hierarchy of interest br22: not printed when high bt warnings are present br24: now high level
</commit_message>
<xml_diff>
--- a/doc/CatalogueBrowser_business_rules_v2.xlsx
+++ b/doc/CatalogueBrowser_business_rules_v2.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23107"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23127"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shahaal\AppData\Local\Eclipse\java_workspace\catalogue-browser\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\eclipse_workspace\cb_workspace\catalogue-browser\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="285" documentId="13_ncr:1_{95F4266B-7B6B-40C1-9ED5-F1FF88022DF9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F96C6306-1428-4984-B6F9-A8872490DD29}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C99DF7C0-3516-4919-B898-504D56915CD7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3912" yWindow="2004" windowWidth="17880" windowHeight="9840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="warningMessages" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -170,15 +170,9 @@
     <t>BR08</t>
   </si>
   <si>
-    <t>The use of not reportable terms is forbidden</t>
-  </si>
-  <si>
     <t>The use of not reportable terms is forbidden.</t>
   </si>
   <si>
-    <t>B09</t>
-  </si>
-  <si>
     <t>BR10</t>
   </si>
   <si>
@@ -377,9 +371,6 @@
     <t>BR23</t>
   </si>
   <si>
-    <t>if a hierarchy is selected as base term</t>
-  </si>
-  <si>
     <t>The use of hierarchy terms as base term is discouraged.</t>
   </si>
   <si>
@@ -498,13 +489,22 @@
   </si>
   <si>
     <t>The facet is not valid for the facet category.</t>
+  </si>
+  <si>
+    <t>BR09</t>
+  </si>
+  <si>
+    <t>warn when selected a term not reportable in the current hierarchy (any hierarchy)</t>
+  </si>
+  <si>
+    <t>if a hierarchy is selected as base term in the exposure</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1274,29 +1274,29 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="34" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="34" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1530,23 +1530,23 @@
       </border>
     </dxf>
     <dxf>
-      <border>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
+      <border>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -1665,7 +1665,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A2:J33" totalsRowShown="0" headerRowDxfId="13" headerRowBorderDxfId="11" tableBorderDxfId="12" totalsRowBorderDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A2:J33" totalsRowShown="0" headerRowDxfId="13" headerRowBorderDxfId="12" tableBorderDxfId="11" totalsRowBorderDxfId="10">
+  <autoFilter ref="A2:J33" xr:uid="{4D34D52D-4A90-49E4-9A08-537EAC2974D7}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Business rule_x000a_code" dataDxfId="9"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Rule Description" dataDxfId="8"/>
@@ -2006,31 +2007,31 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.140625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="50.28515625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="17.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.109375" style="4" customWidth="1"/>
+    <col min="3" max="3" width="50.33203125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="13.88671875" style="2" customWidth="1"/>
     <col min="5" max="5" width="8" style="2" customWidth="1"/>
-    <col min="6" max="6" width="7.140625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="19.5703125" style="4" customWidth="1"/>
-    <col min="8" max="8" width="48.28515625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="7.109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="19.5546875" style="4" customWidth="1"/>
+    <col min="8" max="8" width="48.33203125" style="4" customWidth="1"/>
     <col min="9" max="9" width="39" style="19" customWidth="1"/>
     <col min="10" max="10" width="53" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
-      <c r="G1" s="39" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G1" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="40"/>
-    </row>
-    <row r="2" spans="1:10" s="1" customFormat="1" ht="45">
+      <c r="H1" s="46"/>
+    </row>
+    <row r="2" spans="1:10" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
@@ -2062,7 +2063,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="45">
+    <row r="3" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>11</v>
       </c>
@@ -2090,7 +2091,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>18</v>
       </c>
@@ -2104,7 +2105,7 @@
       <c r="I4" s="10"/>
       <c r="J4" s="35"/>
     </row>
-    <row r="5" spans="1:10" ht="30">
+    <row r="5" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>19</v>
       </c>
@@ -2134,7 +2135,7 @@
       </c>
       <c r="J5" s="18"/>
     </row>
-    <row r="6" spans="1:10" ht="45">
+    <row r="6" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>24</v>
       </c>
@@ -2164,7 +2165,7 @@
       </c>
       <c r="J6" s="18"/>
     </row>
-    <row r="7" spans="1:10" ht="60">
+    <row r="7" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
         <v>29</v>
       </c>
@@ -2194,7 +2195,7 @@
       </c>
       <c r="J7" s="18"/>
     </row>
-    <row r="8" spans="1:10" ht="45">
+    <row r="8" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
         <v>34</v>
       </c>
@@ -2224,7 +2225,7 @@
       </c>
       <c r="J8" s="18"/>
     </row>
-    <row r="9" spans="1:10" ht="75">
+    <row r="9" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
         <v>39</v>
       </c>
@@ -2254,15 +2255,15 @@
       </c>
       <c r="J9" s="18"/>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
         <v>44</v>
       </c>
       <c r="B10" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="C10" s="29" t="s">
         <v>45</v>
-      </c>
-      <c r="C10" s="29" t="s">
-        <v>46</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>14</v>
@@ -2280,9 +2281,9 @@
       <c r="I10" s="16"/>
       <c r="J10" s="18"/>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
-        <v>47</v>
+        <v>152</v>
       </c>
       <c r="B11" s="10"/>
       <c r="C11" s="11"/>
@@ -2294,107 +2295,107 @@
       <c r="I11" s="10"/>
       <c r="J11" s="35"/>
     </row>
-    <row r="12" spans="1:10" ht="30">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" s="29" t="s">
         <v>48</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="C12" s="29" t="s">
-        <v>50</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>14</v>
       </c>
       <c r="E12" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="H12" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="I12" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="G12" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="H12" s="10" t="s">
+      <c r="J12" s="18"/>
+    </row>
+    <row r="13" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="I12" s="16" t="s">
+      <c r="B13" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="J12" s="18"/>
-    </row>
-    <row r="13" spans="1:10" ht="30">
-      <c r="A13" s="9" t="s">
+      <c r="C13" s="29" t="s">
         <v>55</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="C13" s="29" t="s">
-        <v>57</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>14</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H13" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="I13" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="J13" s="18"/>
+    </row>
+    <row r="14" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="I13" s="16" t="s">
+      <c r="B14" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="J13" s="18"/>
-    </row>
-    <row r="14" spans="1:10" ht="45">
-      <c r="A14" s="9" t="s">
+      <c r="C14" s="29" t="s">
         <v>60</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="C14" s="29" t="s">
-        <v>62</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>14</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H14" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="I14" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="J14" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="I14" s="16" t="s">
+    </row>
+    <row r="15" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A15" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="J14" s="18" t="s">
+      <c r="B15" s="13" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" ht="45">
-      <c r="A15" s="32" t="s">
+      <c r="C15" s="31" t="s">
         <v>66</v>
-      </c>
-      <c r="B15" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="C15" s="31" t="s">
-        <v>68</v>
       </c>
       <c r="D15" s="15" t="s">
         <v>14</v>
@@ -2406,79 +2407,79 @@
         <v>15</v>
       </c>
       <c r="G15" s="15" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H15" s="33"/>
       <c r="I15" s="33"/>
       <c r="J15" s="27" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" s="34" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A16" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="B16" s="21" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" s="34" customFormat="1" ht="45">
-      <c r="A16" s="22" t="s">
+      <c r="C16" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="B16" s="21" t="s">
+      <c r="D16" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="C16" s="29" t="s">
+      <c r="E16" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="F16" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="D16" s="23" t="s">
+      <c r="G16" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="H16" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="E16" s="23" t="s">
-        <v>51</v>
-      </c>
-      <c r="F16" s="23" t="s">
+      <c r="I16" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="G16" s="23" t="s">
-        <v>52</v>
-      </c>
-      <c r="H16" s="21" t="s">
+      <c r="J16" s="25"/>
+    </row>
+    <row r="17" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="I16" s="24" t="s">
+      <c r="B17" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="J16" s="25"/>
-    </row>
-    <row r="17" spans="1:10" ht="30">
-      <c r="A17" s="9" t="s">
+      <c r="C17" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="D17" s="5" t="s">
         <v>79</v>
-      </c>
-      <c r="C17" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>81</v>
       </c>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
       <c r="G17" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H17" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="I17" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="J17" s="18"/>
+    </row>
+    <row r="18" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="I17" s="16" t="s">
+      <c r="B18" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="J17" s="18"/>
-    </row>
-    <row r="18" spans="1:10" ht="30">
-      <c r="A18" s="9" t="s">
+      <c r="C18" s="29" t="s">
         <v>84</v>
-      </c>
-      <c r="B18" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="C18" s="29" t="s">
-        <v>86</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>14</v>
@@ -2490,27 +2491,27 @@
         <v>15</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H18" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="I18" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="J18" s="30" t="s">
         <v>87</v>
       </c>
-      <c r="I18" s="16" t="s">
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="J18" s="30" t="s">
+      <c r="B19" s="21" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="19" spans="1:10">
-      <c r="A19" s="9" t="s">
+      <c r="C19" s="29" t="s">
         <v>90</v>
-      </c>
-      <c r="B19" s="21" t="s">
-        <v>91</v>
-      </c>
-      <c r="C19" s="29" t="s">
-        <v>92</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>14</v>
@@ -2522,17 +2523,17 @@
         <v>15</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H19" s="10" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="I19" s="16"/>
       <c r="J19" s="18"/>
     </row>
-    <row r="20" spans="1:10" s="34" customFormat="1">
+    <row r="20" spans="1:10" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="32" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B20" s="33"/>
       <c r="C20" s="36"/>
@@ -2544,15 +2545,15 @@
       <c r="I20" s="38"/>
       <c r="J20" s="38"/>
     </row>
-    <row r="21" spans="1:10" ht="45">
+    <row r="21" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A21" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="B21" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="C21" s="29" t="s">
         <v>95</v>
-      </c>
-      <c r="B21" s="21" t="s">
-        <v>96</v>
-      </c>
-      <c r="C21" s="29" t="s">
-        <v>97</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>14</v>
@@ -2564,27 +2565,27 @@
         <v>15</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H21" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="I21" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="J21" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="I21" s="16" t="s">
+    </row>
+    <row r="22" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A22" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="J21" s="18" t="s">
+      <c r="B22" s="10" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" ht="30">
-      <c r="A22" s="9" t="s">
+      <c r="C22" s="29" t="s">
         <v>101</v>
-      </c>
-      <c r="B22" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="C22" s="29" t="s">
-        <v>103</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>14</v>
@@ -2596,29 +2597,29 @@
         <v>15</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H22" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="I22" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="J22" s="18"/>
+    </row>
+    <row r="23" spans="1:10" s="26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="22" t="s">
         <v>104</v>
       </c>
-      <c r="I22" s="16" t="s">
+      <c r="B23" s="21" t="s">
         <v>105</v>
       </c>
-      <c r="J22" s="18"/>
-    </row>
-    <row r="23" spans="1:10" s="26" customFormat="1" ht="30">
-      <c r="A23" s="22" t="s">
+      <c r="C23" s="29" t="s">
         <v>106</v>
       </c>
-      <c r="B23" s="21" t="s">
+      <c r="D23" s="23" t="s">
         <v>107</v>
       </c>
-      <c r="C23" s="29" t="s">
-        <v>108</v>
-      </c>
-      <c r="D23" s="23" t="s">
-        <v>109</v>
-      </c>
       <c r="E23" s="23" t="s">
         <v>15</v>
       </c>
@@ -2626,7 +2627,7 @@
         <v>15</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H23" s="21"/>
       <c r="I23" s="24"/>
@@ -2634,100 +2635,100 @@
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="C24" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="B24" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="C24" s="11" t="s">
-        <v>112</v>
-      </c>
       <c r="D24" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G24" s="5"/>
       <c r="H24" s="10"/>
       <c r="I24" s="16"/>
       <c r="J24" s="18"/>
     </row>
-    <row r="25" spans="1:10" ht="30">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="9" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>114</v>
+        <v>154</v>
       </c>
       <c r="C25" s="29" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D25" s="5" t="s">
         <v>14</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H25" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="I25" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="J25" s="30"/>
+    </row>
+    <row r="26" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A26" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="B26" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="I25" s="16" t="s">
+      <c r="C26" s="29" t="s">
         <v>117</v>
       </c>
-      <c r="J25" s="30"/>
-    </row>
-    <row r="26" spans="1:10" ht="30">
-      <c r="A26" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="B26" s="10" t="s">
-        <v>119</v>
-      </c>
-      <c r="C26" s="29" t="s">
-        <v>120</v>
-      </c>
       <c r="D26" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G26" s="5"/>
       <c r="H26" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="I26" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="J26" s="18"/>
+    </row>
+    <row r="27" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A27" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="B27" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="I26" s="16" t="s">
+      <c r="C27" s="29" t="s">
         <v>122</v>
       </c>
-      <c r="J26" s="18"/>
-    </row>
-    <row r="27" spans="1:10" ht="30">
-      <c r="A27" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="B27" s="10" t="s">
-        <v>124</v>
-      </c>
-      <c r="C27" s="29" t="s">
-        <v>125</v>
-      </c>
       <c r="D27" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E27" s="5" t="s">
         <v>15</v>
@@ -2739,57 +2740,57 @@
         <v>16</v>
       </c>
       <c r="H27" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="I27" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="J27" s="30" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A28" s="39" t="s">
         <v>126</v>
       </c>
-      <c r="I27" s="16" t="s">
+      <c r="B28" s="40" t="s">
         <v>127</v>
       </c>
-      <c r="J27" s="30" t="s">
+      <c r="C28" s="41" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" ht="30">
-      <c r="A28" s="41" t="s">
+      <c r="D28" s="42" t="s">
+        <v>107</v>
+      </c>
+      <c r="E28" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="F28" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="G28" s="42"/>
+      <c r="H28" s="40" t="s">
         <v>129</v>
       </c>
-      <c r="B28" s="42" t="s">
+      <c r="I28" s="43" t="s">
         <v>130</v>
       </c>
-      <c r="C28" s="43" t="s">
+      <c r="J28" s="44" t="s">
         <v>131</v>
       </c>
-      <c r="D28" s="44" t="s">
-        <v>109</v>
-      </c>
-      <c r="E28" s="44" t="s">
-        <v>15</v>
-      </c>
-      <c r="F28" s="44" t="s">
-        <v>15</v>
-      </c>
-      <c r="G28" s="44"/>
-      <c r="H28" s="42" t="s">
+    </row>
+    <row r="29" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A29" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="I28" s="45" t="s">
+      <c r="B29" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="J28" s="46" t="s">
+      <c r="C29" s="29" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" ht="45">
-      <c r="A29" s="9" t="s">
-        <v>135</v>
-      </c>
-      <c r="B29" s="10" t="s">
-        <v>136</v>
-      </c>
-      <c r="C29" s="29" t="s">
-        <v>137</v>
-      </c>
       <c r="D29" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E29" s="5" t="s">
         <v>15</v>
@@ -2799,25 +2800,25 @@
       </c>
       <c r="G29" s="5"/>
       <c r="H29" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="I29" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="J29" s="18"/>
+    </row>
+    <row r="30" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A30" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="B30" s="10" t="s">
         <v>138</v>
       </c>
-      <c r="I29" s="16" t="s">
+      <c r="C30" s="29" t="s">
         <v>139</v>
       </c>
-      <c r="J29" s="18"/>
-    </row>
-    <row r="30" spans="1:10" ht="45">
-      <c r="A30" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="B30" s="10" t="s">
-        <v>141</v>
-      </c>
-      <c r="C30" s="29" t="s">
-        <v>142</v>
-      </c>
       <c r="D30" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E30" s="5" t="s">
         <v>15</v>
@@ -2827,81 +2828,81 @@
       </c>
       <c r="G30" s="5"/>
       <c r="H30" s="10" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="I30" s="16" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="J30" s="18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="30">
+    <row r="31" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A31" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="D31" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="B31" s="10" t="s">
-        <v>146</v>
-      </c>
-      <c r="C31" s="11" t="s">
-        <v>147</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>148</v>
-      </c>
       <c r="E31" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G31" s="5"/>
       <c r="H31" s="10"/>
       <c r="I31" s="16"/>
       <c r="J31" s="18"/>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" s="9" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G32" s="5"/>
       <c r="H32" s="10"/>
       <c r="I32" s="16"/>
       <c r="J32" s="18"/>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" s="12" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="D33" s="15" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E33" s="15" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F33" s="15" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G33" s="15"/>
       <c r="H33" s="13"/>
@@ -2950,12 +2951,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BD575A271421684D80D50334C5201F8B" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d0f74c06de7f9d11e163ca3490207ad2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9fa0de94-d05f-4933-bc1c-54b600203760" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="519e242d08df03fdeb2dcdffae48ed89" ns2:_="">
     <xsd:import namespace="9fa0de94-d05f-4933-bc1c-54b600203760"/>
@@ -3113,6 +3108,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -3123,13 +3124,36 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B31F279E-4409-453A-A730-B0F4195EDC04}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{174CF0A8-FB3C-428C-A2EF-83C3FD6050DE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="9fa0de94-d05f-4933-bc1c-54b600203760"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{174CF0A8-FB3C-428C-A2EF-83C3FD6050DE}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B31F279E-4409-453A-A730-B0F4195EDC04}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DCDD3505-D720-4670-82CB-1CB7793CB735}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DCDD3505-D720-4670-82CB-1CB7793CB735}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>